<commit_message>
overview generated for the closing 2023
</commit_message>
<xml_diff>
--- a/data/dataverse_absolute.xlsx
+++ b/data/dataverse_absolute.xlsx
@@ -501,7 +501,7 @@
         <v>2</v>
       </c>
       <c r="K2">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -536,7 +536,7 @@
         <v>1</v>
       </c>
       <c r="K3">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -571,7 +571,7 @@
         <v>17</v>
       </c>
       <c r="K4">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:11">
@@ -606,7 +606,7 @@
         <v>36</v>
       </c>
       <c r="K5">
-        <v>6</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:11">

</xml_diff>